<commit_message>
Deleted redundant files. Renamed testing script. Finalized process as function: 'ValveTimingFunc'. Added necessary .xlsx files to project folder. Ready for review.
</commit_message>
<xml_diff>
--- a/Valve Timing Script/ValveTimingTestResults.xlsx
+++ b/Valve Timing Script/ValveTimingTestResults.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="213" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="182" uniqueCount="50">
   <si>
     <t>Valve Type</t>
   </si>
@@ -175,15 +175,6 @@
   </si>
   <si>
     <t>15C313</t>
-  </si>
-  <si>
-    <t>The following I/O Codes are missing data:NaN</t>
-  </si>
-  <si>
-    <t>The following I/O Codes are missing data:,NaN,NaN</t>
-  </si>
-  <si>
-    <t>Datum times are inconsistent across data. Cannot compute timing.</t>
   </si>
 </sst>
 </file>
@@ -679,7 +670,7 @@
   <cols>
     <col min="1" max="1" width="10.85546875" style="4" customWidth="true"/>
     <col min="3" max="3" width="13.5703125" style="4" customWidth="true"/>
-    <col min="5" max="5" width="59.42578125" style="11" customWidth="true"/>
+    <col min="5" max="5" width="6.28515625" style="11" customWidth="true"/>
     <col min="6" max="16384" width="9.140625" style="4"/>
     <col min="2" max="2" width="9" style="4" customWidth="true"/>
     <col min="4" max="4" width="13.5703125" style="4" customWidth="true"/>
@@ -709,11 +700,13 @@
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C2" s="12">
+        <v>1.4666666666666668</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1.8666666666666669</v>
+      </c>
+      <c r="E2" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -722,11 +715,13 @@
       <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C3" s="14">
+        <v>2</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="E3" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -735,11 +730,13 @@
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C4" s="12">
+        <v>2.2333333333333334</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.56666666666666676</v>
+      </c>
+      <c r="E4" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -748,11 +745,13 @@
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C5" s="14">
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="E5" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -761,11 +760,13 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C6" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D6" s="13">
+        <v>2.2666666666666671</v>
+      </c>
+      <c r="E6" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -774,11 +775,13 @@
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C7" s="14">
+        <v>1.3</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="E7" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -787,11 +790,13 @@
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C8" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="E8" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -800,11 +805,13 @@
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C9" s="14">
+        <v>2.4333333333333336</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -813,11 +820,13 @@
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C10" s="12">
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1.9666666666666668</v>
+      </c>
+      <c r="E10" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -886,11 +895,13 @@
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C15" s="14">
+        <v>1.6333333333333335</v>
+      </c>
+      <c r="D15" s="15">
+        <v>7.5333333333333341</v>
+      </c>
+      <c r="E15" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -914,11 +925,13 @@
       <c r="B17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C17" s="14">
+        <v>1.7666666666666668</v>
+      </c>
+      <c r="D17" s="15">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="E17" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -927,11 +940,13 @@
       <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C18" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -970,11 +985,13 @@
       <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="11" t="s">
-        <v>52</v>
-      </c>
+      <c r="C21" s="14">
+        <v>1.5333333333333332</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="E21" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1013,11 +1030,13 @@
       <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C24" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E24" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1041,11 +1060,13 @@
       <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="C26" s="12">
+        <v>1.4666666666666668</v>
+      </c>
+      <c r="D26" s="13">
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="E26" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -1084,11 +1105,13 @@
       <c r="B29" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C29" s="14">
+        <v>0</v>
+      </c>
+      <c r="D29" s="15">
+        <v>0</v>
+      </c>
+      <c r="E29" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -1097,11 +1120,13 @@
       <c r="B30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C30" s="12">
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="D30" s="13">
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="E30" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -1110,11 +1135,13 @@
       <c r="B31" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C31" s="14">
+        <v>0.23333333333333331</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="E31" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="32" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -1123,11 +1150,13 @@
       <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C32" s="12">
+        <v>0</v>
+      </c>
+      <c r="D32" s="13">
+        <v>0</v>
+      </c>
+      <c r="E32" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="33" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -1136,11 +1165,13 @@
       <c r="B33" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C33" s="14">
+        <v>0</v>
+      </c>
+      <c r="D33" s="15">
+        <v>0</v>
+      </c>
+      <c r="E33" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="34" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
@@ -1149,11 +1180,13 @@
       <c r="B34" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C34" s="12">
+        <v>0</v>
+      </c>
+      <c r="D34" s="13">
+        <v>0</v>
+      </c>
+      <c r="E34" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="35" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -1162,11 +1195,13 @@
       <c r="B35" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C35" s="14">
+        <v>0</v>
+      </c>
+      <c r="D35" s="15">
+        <v>0</v>
+      </c>
+      <c r="E35" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="36" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -1175,11 +1210,13 @@
       <c r="B36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C36" s="12">
+        <v>0</v>
+      </c>
+      <c r="D36" s="13">
+        <v>0</v>
+      </c>
+      <c r="E36" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="37" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -1188,11 +1225,13 @@
       <c r="B37" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C37" s="14">
+        <v>0</v>
+      </c>
+      <c r="D37" s="15">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="38" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1201,11 +1240,13 @@
       <c r="B38" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C38" s="12">
+        <v>0</v>
+      </c>
+      <c r="D38" s="13">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="39" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
@@ -1214,11 +1255,13 @@
       <c r="B39" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C39" s="14">
+        <v>0</v>
+      </c>
+      <c r="D39" s="15">
+        <v>0</v>
+      </c>
+      <c r="E39" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="40" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -1227,11 +1270,13 @@
       <c r="B40" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C40" s="12">
+        <v>0</v>
+      </c>
+      <c r="D40" s="13">
+        <v>0</v>
+      </c>
+      <c r="E40" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="41" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
@@ -1240,11 +1285,13 @@
       <c r="B41" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C41" s="14">
+        <v>0</v>
+      </c>
+      <c r="D41" s="15">
+        <v>0</v>
+      </c>
+      <c r="E41" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="42" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1253,11 +1300,13 @@
       <c r="B42" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C42" s="12">
+        <v>0</v>
+      </c>
+      <c r="D42" s="13">
+        <v>0</v>
+      </c>
+      <c r="E42" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="43" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
@@ -1266,11 +1315,13 @@
       <c r="B43" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C43" s="14">
+        <v>0</v>
+      </c>
+      <c r="D43" s="15">
+        <v>0</v>
+      </c>
+      <c r="E43" s="11"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="44" ht="15.75" thickBot="true" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
@@ -1279,11 +1330,13 @@
       <c r="B44" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="C44" s="16">
+        <v>0</v>
+      </c>
+      <c r="D44" s="17">
+        <v>0</v>
+      </c>
+      <c r="E44" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>